<commit_message>
batch updates from shell script..
</commit_message>
<xml_diff>
--- a/trailtech/Leistungen-KC-Trailtech.xlsx
+++ b/trailtech/Leistungen-KC-Trailtech.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="858">
   <si>
     <t>Tätigkeit</t>
   </si>
@@ -2649,9 +2649,6 @@
     <t>Talks with David on Appo</t>
   </si>
   <si>
-    <t>Thomas Falkner Update -&gt; Gem.sitzung Mils smid January -&gt; hopefully commitment by the Gemeinde. BGm is fully committed;)</t>
-  </si>
-  <si>
     <t>Jochtal-Gitschberg</t>
   </si>
   <si>
@@ -2665,6 +2662,42 @@
 Viktoria Leitner (Gitschberg Jochtal AG Büroleitung)
 Markus Reifer (Ski- &amp; Almenregion Gitschberg Jochtal Buchhaltung)
 Stefan Gruber (Gitschberg Jochtal AG GF)</t>
+  </si>
+  <si>
+    <t>Dezember (Rechnung fehlt noch)</t>
+  </si>
+  <si>
+    <t>VS Graz</t>
+  </si>
+  <si>
+    <t>Uli Absprache</t>
+  </si>
+  <si>
+    <t>Marina E-Mails</t>
+  </si>
+  <si>
+    <t>Absprache Cody</t>
+  </si>
+  <si>
+    <t>Anlage Projektdateien in GD</t>
+  </si>
+  <si>
+    <t>Konrad neue Rechnungsadresse</t>
+  </si>
+  <si>
+    <t>Polak Rechnungsübermittlung</t>
+  </si>
+  <si>
+    <t>Thomas Falkner Update -&gt; Gem.sitzung Mils mid January -&gt; hopefully commitment by the Gemeinde. BGm is fully committed;)</t>
+  </si>
+  <si>
+    <t>Referenzen neu übermitteln</t>
+  </si>
+  <si>
+    <t>Referenzen neu, Auswahl Fotos, Text, Einarbeitung</t>
+  </si>
+  <si>
+    <t>Termin Akk.</t>
   </si>
 </sst>
 </file>
@@ -3483,246 +3516,6 @@
   <dxfs count="107">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3990,6 +3783,246 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5347,29 +5380,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TAB_Doku_201910" displayName="TAB_Doku_201910" ref="A1:H56" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49" tableBorderDxfId="48">
-  <autoFilter ref="A1:H55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TAB_Doku_201910" displayName="TAB_Doku_201910" ref="A1:H65" totalsRowCount="1" headerRowDxfId="51" dataDxfId="50" totalsRowDxfId="49" tableBorderDxfId="48">
+  <autoFilter ref="A1:H64">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:H55">
     <sortCondition ref="C1:C55"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Projekt" totalsRowLabel="SUMME für Zeitraum Leistungszeitraum von-bis" dataDxfId="47" totalsRowDxfId="31"/>
-    <tableColumn id="2" name="Leistung" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="30">
+    <tableColumn id="1" name="Projekt" totalsRowLabel="SUMME für Zeitraum Leistungszeitraum von-bis" dataDxfId="47" totalsRowDxfId="7"/>
+    <tableColumn id="2" name="Leistung" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="6">
       <totalsRowFormula>SUBTOTAL(5,TAB_Doku_201910[Datum])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Datum" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="29">
+    <tableColumn id="3" name="Datum" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="5">
       <totalsRowFormula>SUBTOTAL(4,TAB_Doku_201910[Datum])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Stk." dataDxfId="44" totalsRowDxfId="28"/>
-    <tableColumn id="5" name="Zeitaufwand" dataDxfId="43" totalsRowDxfId="27">
+    <tableColumn id="4" name="Stk." dataDxfId="44" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Zeitaufwand" dataDxfId="43" totalsRowDxfId="3">
       <calculatedColumnFormula>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Kosten " totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="26">
+    <tableColumn id="6" name="Kosten " totalsRowFunction="custom" dataDxfId="42" totalsRowDxfId="2">
       <calculatedColumnFormula>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</calculatedColumnFormula>
       <totalsRowFormula>SUBTOTAL(9,TAB_Doku_201910[[Kosten ]])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="Abrechnung" dataDxfId="41" totalsRowDxfId="25"/>
-    <tableColumn id="8" name="Notiz" dataDxfId="40" totalsRowDxfId="24"/>
+    <tableColumn id="7" name="Abrechnung" dataDxfId="41" totalsRowDxfId="1"/>
+    <tableColumn id="8" name="Notiz" dataDxfId="40" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6737,13 +6776,13 @@
   <sheetPr published="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I313"/>
+  <dimension ref="A1:I322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6785,181 +6824,181 @@
     </row>
     <row r="2" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="78" t="s">
-        <v>816</v>
+        <v>847</v>
       </c>
       <c r="B2" s="133" t="s">
-        <v>140</v>
+        <v>48</v>
       </c>
       <c r="C2" s="137">
-        <v>44201</v>
+        <v>44208</v>
       </c>
       <c r="D2" s="133">
         <v>3</v>
       </c>
       <c r="E2" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F2" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>7.5</v>
+        <v>22.5</v>
       </c>
       <c r="G2" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H2" s="134" t="s">
-        <v>840</v>
+        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="s">
-        <v>744</v>
-      </c>
-      <c r="B3" s="132" t="s">
-        <v>1</v>
+        <v>830</v>
+      </c>
+      <c r="B3" s="133" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="137">
-        <v>44201</v>
+        <v>44209</v>
       </c>
       <c r="D3" s="133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="G3" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H3" s="134" t="s">
-        <v>841</v>
+        <v>857</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="78" t="s">
-        <v>830</v>
-      </c>
-      <c r="B4" s="132" t="s">
-        <v>48</v>
+        <v>847</v>
+      </c>
+      <c r="B4" s="133" t="s">
+        <v>140</v>
       </c>
       <c r="C4" s="137">
-        <v>44201</v>
+        <v>44209</v>
       </c>
       <c r="D4" s="133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F4" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="G4" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H4" s="134" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="78" t="s">
-        <v>843</v>
-      </c>
-      <c r="B5" s="132" t="s">
-        <v>48</v>
+        <v>847</v>
+      </c>
+      <c r="B5" s="133" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="137">
-        <v>44203</v>
+        <v>44210</v>
       </c>
       <c r="D5" s="133">
         <v>1</v>
       </c>
       <c r="E5" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F5" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>7.5</v>
+        <v>30</v>
       </c>
       <c r="G5" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H5" s="134" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="78" t="s">
-        <v>780</v>
-      </c>
-      <c r="B6" s="132" t="s">
-        <v>1</v>
+        <v>847</v>
+      </c>
+      <c r="B6" s="133" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="137">
-        <v>44203</v>
+        <v>44210</v>
       </c>
       <c r="D6" s="133">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F6" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G6" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H6" s="134" t="s">
-        <v>842</v>
+        <v>851</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="78" t="s">
-        <v>816</v>
-      </c>
-      <c r="B7" s="132" t="s">
-        <v>1</v>
+        <v>727</v>
+      </c>
+      <c r="B7" s="133" t="s">
+        <v>140</v>
       </c>
       <c r="C7" s="137">
-        <v>44203</v>
+        <v>44209</v>
       </c>
       <c r="D7" s="133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F7" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="G7" s="78" t="s">
         <v>498</v>
       </c>
       <c r="H7" s="134" t="s">
-        <v>839</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="78" t="s">
-        <v>781</v>
-      </c>
-      <c r="B8" s="132" t="s">
+        <v>727</v>
+      </c>
+      <c r="B8" s="133" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="137">
-        <v>44203</v>
+        <v>44209</v>
       </c>
       <c r="D8" s="133">
         <v>1</v>
@@ -6976,18 +7015,18 @@
         <v>498</v>
       </c>
       <c r="H8" s="134" t="s">
-        <v>844</v>
+        <v>853</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="78" t="s">
-        <v>767</v>
-      </c>
-      <c r="B9" s="132" t="s">
+        <v>816</v>
+      </c>
+      <c r="B9" s="133" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="137">
-        <v>44203</v>
+        <v>44209</v>
       </c>
       <c r="D9" s="133">
         <v>1</v>
@@ -7004,174 +7043,264 @@
         <v>498</v>
       </c>
       <c r="H9" s="134" t="s">
-        <v>844</v>
+        <v>855</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="78" t="s">
-        <v>727</v>
-      </c>
-      <c r="B10" s="132"/>
-      <c r="C10" s="137"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133" t="e">
+        <v>102</v>
+      </c>
+      <c r="B10" s="133" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="137">
+        <v>44208</v>
+      </c>
+      <c r="D10" s="133">
+        <v>2</v>
+      </c>
+      <c r="E10" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F10" s="133" t="e">
+        <v>60</v>
+      </c>
+      <c r="F10" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G10" s="78"/>
-      <c r="H10" s="134"/>
+        <v>60</v>
+      </c>
+      <c r="G10" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H10" s="134" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="78" t="s">
-        <v>813</v>
-      </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133" t="e">
+        <v>816</v>
+      </c>
+      <c r="B11" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="137">
+        <v>44201</v>
+      </c>
+      <c r="D11" s="133">
+        <v>3</v>
+      </c>
+      <c r="E11" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F11" s="133" t="e">
+        <v>5</v>
+      </c>
+      <c r="F11" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G11" s="78"/>
-      <c r="H11" s="134"/>
+        <v>7.5</v>
+      </c>
+      <c r="G11" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H11" s="134" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="78" t="s">
-        <v>819</v>
-      </c>
-      <c r="B12" s="132"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133" t="e">
+        <v>744</v>
+      </c>
+      <c r="B12" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="137">
+        <v>44201</v>
+      </c>
+      <c r="D12" s="133">
+        <v>2</v>
+      </c>
+      <c r="E12" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="133" t="e">
+        <v>10</v>
+      </c>
+      <c r="F12" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G12" s="78"/>
-      <c r="H12" s="134"/>
+        <v>10</v>
+      </c>
+      <c r="G12" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H12" s="134" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="78" t="s">
-        <v>810</v>
-      </c>
-      <c r="B13" s="132"/>
-      <c r="C13" s="137"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133" t="e">
+        <v>830</v>
+      </c>
+      <c r="B13" s="132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="137">
+        <v>44201</v>
+      </c>
+      <c r="D13" s="133">
+        <v>1</v>
+      </c>
+      <c r="E13" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="133" t="e">
+        <v>15</v>
+      </c>
+      <c r="F13" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="134"/>
+        <v>7.5</v>
+      </c>
+      <c r="G13" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H13" s="134" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="78" t="s">
-        <v>765</v>
-      </c>
-      <c r="B14" s="132"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133" t="e">
+        <v>842</v>
+      </c>
+      <c r="B14" s="132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="137">
+        <v>44203</v>
+      </c>
+      <c r="D14" s="133">
+        <v>1</v>
+      </c>
+      <c r="E14" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="133" t="e">
+        <v>15</v>
+      </c>
+      <c r="F14" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" s="78"/>
-      <c r="H14" s="134"/>
+        <v>7.5</v>
+      </c>
+      <c r="G14" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H14" s="134" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="78" t="s">
-        <v>795</v>
-      </c>
-      <c r="B15" s="132"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="133" t="e">
+        <v>780</v>
+      </c>
+      <c r="B15" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="137">
+        <v>44203</v>
+      </c>
+      <c r="D15" s="133">
+        <v>1</v>
+      </c>
+      <c r="E15" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="133" t="e">
+        <v>10</v>
+      </c>
+      <c r="F15" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G15" s="78"/>
-      <c r="H15" s="134"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H15" s="134" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="78" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="132"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133" t="e">
+        <v>816</v>
+      </c>
+      <c r="B16" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="137">
+        <v>44203</v>
+      </c>
+      <c r="D16" s="133">
+        <v>2</v>
+      </c>
+      <c r="E16" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="133" t="e">
+        <v>10</v>
+      </c>
+      <c r="F16" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="134"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H16" s="134" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78" t="s">
-        <v>780</v>
-      </c>
-      <c r="B17" s="132"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133" t="e">
+        <v>781</v>
+      </c>
+      <c r="B17" s="132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="137">
+        <v>44203</v>
+      </c>
+      <c r="D17" s="133">
+        <v>1</v>
+      </c>
+      <c r="E17" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F17" s="133" t="e">
+        <v>15</v>
+      </c>
+      <c r="F17" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G17" s="78"/>
-      <c r="H17" s="134"/>
+        <v>7.5</v>
+      </c>
+      <c r="G17" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H17" s="134" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="78" t="s">
-        <v>734</v>
-      </c>
-      <c r="B18" s="132"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133" t="e">
+        <v>767</v>
+      </c>
+      <c r="B18" s="132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="137">
+        <v>44203</v>
+      </c>
+      <c r="D18" s="133">
+        <v>1</v>
+      </c>
+      <c r="E18" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="133" t="e">
+        <v>15</v>
+      </c>
+      <c r="F18" s="133">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G18" s="78"/>
-      <c r="H18" s="134"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+      <c r="G18" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="H18" s="134" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78" t="s">
-        <v>789</v>
+        <v>727</v>
       </c>
       <c r="B19" s="132"/>
       <c r="C19" s="137"/>
@@ -7187,11 +7316,11 @@
       <c r="G19" s="78"/>
       <c r="H19" s="134"/>
     </row>
-    <row r="20" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="78" t="s">
-        <v>760</v>
-      </c>
-      <c r="B20" s="132"/>
+        <v>813</v>
+      </c>
+      <c r="B20" s="133"/>
       <c r="C20" s="137"/>
       <c r="D20" s="133"/>
       <c r="E20" s="133" t="e">
@@ -7205,9 +7334,9 @@
       <c r="G20" s="78"/>
       <c r="H20" s="134"/>
     </row>
-    <row r="21" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="78" t="s">
-        <v>738</v>
+        <v>819</v>
       </c>
       <c r="B21" s="132"/>
       <c r="C21" s="137"/>
@@ -7223,9 +7352,9 @@
       <c r="G21" s="78"/>
       <c r="H21" s="134"/>
     </row>
-    <row r="22" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="78" t="s">
-        <v>756</v>
+        <v>810</v>
       </c>
       <c r="B22" s="132"/>
       <c r="C22" s="137"/>
@@ -7241,9 +7370,9 @@
       <c r="G22" s="78"/>
       <c r="H22" s="134"/>
     </row>
-    <row r="23" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="78" t="s">
-        <v>728</v>
+        <v>765</v>
       </c>
       <c r="B23" s="132"/>
       <c r="C23" s="137"/>
@@ -7259,9 +7388,9 @@
       <c r="G23" s="78"/>
       <c r="H23" s="134"/>
     </row>
-    <row r="24" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="78" t="s">
-        <v>725</v>
+        <v>795</v>
       </c>
       <c r="B24" s="132"/>
       <c r="C24" s="137"/>
@@ -7277,9 +7406,9 @@
       <c r="G24" s="78"/>
       <c r="H24" s="134"/>
     </row>
-    <row r="25" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="78" t="s">
-        <v>726</v>
+        <v>102</v>
       </c>
       <c r="B25" s="132"/>
       <c r="C25" s="137"/>
@@ -7295,9 +7424,9 @@
       <c r="G25" s="78"/>
       <c r="H25" s="134"/>
     </row>
-    <row r="26" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="78" t="s">
-        <v>672</v>
+        <v>780</v>
       </c>
       <c r="B26" s="132"/>
       <c r="C26" s="137"/>
@@ -7313,9 +7442,9 @@
       <c r="G26" s="78"/>
       <c r="H26" s="134"/>
     </row>
-    <row r="27" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="78" t="s">
-        <v>631</v>
+        <v>734</v>
       </c>
       <c r="B27" s="132"/>
       <c r="C27" s="137"/>
@@ -7328,12 +7457,12 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G27" s="130"/>
+      <c r="G27" s="78"/>
       <c r="H27" s="134"/>
     </row>
-    <row r="28" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="78" t="s">
-        <v>509</v>
+        <v>789</v>
       </c>
       <c r="B28" s="132"/>
       <c r="C28" s="137"/>
@@ -7349,9 +7478,9 @@
       <c r="G28" s="78"/>
       <c r="H28" s="134"/>
     </row>
-    <row r="29" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="78" t="s">
-        <v>643</v>
+        <v>760</v>
       </c>
       <c r="B29" s="132"/>
       <c r="C29" s="137"/>
@@ -7367,9 +7496,9 @@
       <c r="G29" s="78"/>
       <c r="H29" s="134"/>
     </row>
-    <row r="30" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78" t="s">
-        <v>649</v>
+        <v>738</v>
       </c>
       <c r="B30" s="132"/>
       <c r="C30" s="137"/>
@@ -7385,9 +7514,9 @@
       <c r="G30" s="78"/>
       <c r="H30" s="134"/>
     </row>
-    <row r="31" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
-        <v>642</v>
+        <v>756</v>
       </c>
       <c r="B31" s="132"/>
       <c r="C31" s="137"/>
@@ -7403,12 +7532,12 @@
       <c r="G31" s="78"/>
       <c r="H31" s="134"/>
     </row>
-    <row r="32" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="147" t="s">
-        <v>609</v>
+    <row r="32" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="78" t="s">
+        <v>728</v>
       </c>
       <c r="B32" s="132"/>
-      <c r="C32" s="149"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="133"/>
       <c r="E32" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
@@ -7418,16 +7547,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G32" s="130"/>
-      <c r="H32" s="138"/>
-    </row>
-    <row r="33" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="78"/>
+      <c r="H32" s="134"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="78" t="s">
-        <v>640</v>
+        <v>725</v>
       </c>
       <c r="B33" s="132"/>
-      <c r="C33" s="149"/>
-      <c r="D33" s="138"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="133"/>
       <c r="E33" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7436,16 +7565,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G33" s="130"/>
-      <c r="H33" s="148"/>
-    </row>
-    <row r="34" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="147" t="s">
-        <v>607</v>
+      <c r="G33" s="78"/>
+      <c r="H33" s="134"/>
+    </row>
+    <row r="34" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="78" t="s">
+        <v>726</v>
       </c>
       <c r="B34" s="132"/>
-      <c r="C34" s="149"/>
-      <c r="D34" s="138"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="133"/>
       <c r="E34" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7454,16 +7583,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="148"/>
-    </row>
-    <row r="35" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="147" t="s">
-        <v>597</v>
+      <c r="G34" s="78"/>
+      <c r="H34" s="134"/>
+    </row>
+    <row r="35" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="78" t="s">
+        <v>672</v>
       </c>
       <c r="B35" s="132"/>
-      <c r="C35" s="149"/>
-      <c r="D35" s="138"/>
+      <c r="C35" s="137"/>
+      <c r="D35" s="133"/>
       <c r="E35" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7472,16 +7601,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G35" s="130"/>
-      <c r="H35" s="148"/>
-    </row>
-    <row r="36" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="147" t="s">
-        <v>500</v>
+      <c r="G35" s="78"/>
+      <c r="H35" s="134"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="78" t="s">
+        <v>631</v>
       </c>
       <c r="B36" s="132"/>
-      <c r="C36" s="149"/>
-      <c r="D36" s="138"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="133"/>
       <c r="E36" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7491,15 +7620,15 @@
         <v>#N/A</v>
       </c>
       <c r="G36" s="130"/>
-      <c r="H36" s="148"/>
-    </row>
-    <row r="37" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="130" t="s">
-        <v>278</v>
+      <c r="H36" s="134"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="78" t="s">
+        <v>509</v>
       </c>
       <c r="B37" s="132"/>
-      <c r="C37" s="149"/>
-      <c r="D37" s="138"/>
+      <c r="C37" s="137"/>
+      <c r="D37" s="133"/>
       <c r="E37" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7508,16 +7637,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G37" s="130"/>
-      <c r="H37" s="148"/>
-    </row>
-    <row r="38" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="147" t="s">
-        <v>593</v>
+      <c r="G37" s="78"/>
+      <c r="H37" s="134"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="78" t="s">
+        <v>643</v>
       </c>
       <c r="B38" s="132"/>
-      <c r="C38" s="149"/>
-      <c r="D38" s="138"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="133"/>
       <c r="E38" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7526,16 +7655,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G38" s="130"/>
-      <c r="H38" s="148"/>
-    </row>
-    <row r="39" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="147" t="s">
-        <v>574</v>
+      <c r="G38" s="78"/>
+      <c r="H38" s="134"/>
+    </row>
+    <row r="39" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="78" t="s">
+        <v>649</v>
       </c>
       <c r="B39" s="132"/>
-      <c r="C39" s="149"/>
-      <c r="D39" s="138"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="133"/>
       <c r="E39" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7544,16 +7673,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G39" s="130"/>
-      <c r="H39" s="148"/>
-    </row>
-    <row r="40" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="147" t="s">
-        <v>178</v>
+      <c r="G39" s="78"/>
+      <c r="H39" s="134"/>
+    </row>
+    <row r="40" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="78" t="s">
+        <v>642</v>
       </c>
       <c r="B40" s="132"/>
-      <c r="C40" s="149"/>
-      <c r="D40" s="138"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="133"/>
       <c r="E40" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7562,16 +7691,16 @@
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
         <v>#N/A</v>
       </c>
-      <c r="G40" s="130"/>
-      <c r="H40" s="148"/>
-    </row>
-    <row r="41" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="78"/>
+      <c r="H40" s="134"/>
+    </row>
+    <row r="41" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="147" t="s">
-        <v>576</v>
+        <v>609</v>
       </c>
       <c r="B41" s="132"/>
       <c r="C41" s="149"/>
-      <c r="D41" s="138"/>
+      <c r="D41" s="133"/>
       <c r="E41" s="133" t="e">
         <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
         <v>#N/A</v>
@@ -7581,11 +7710,11 @@
         <v>#N/A</v>
       </c>
       <c r="G41" s="130"/>
-      <c r="H41" s="148"/>
-    </row>
-    <row r="42" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="147" t="s">
-        <v>541</v>
+      <c r="H41" s="138"/>
+    </row>
+    <row r="42" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="78" t="s">
+        <v>640</v>
       </c>
       <c r="B42" s="132"/>
       <c r="C42" s="149"/>
@@ -7601,9 +7730,9 @@
       <c r="G42" s="130"/>
       <c r="H42" s="148"/>
     </row>
-    <row r="43" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="147" t="s">
-        <v>239</v>
+        <v>607</v>
       </c>
       <c r="B43" s="132"/>
       <c r="C43" s="149"/>
@@ -7619,9 +7748,9 @@
       <c r="G43" s="130"/>
       <c r="H43" s="148"/>
     </row>
-    <row r="44" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="130" t="s">
-        <v>492</v>
+    <row r="44" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="147" t="s">
+        <v>597</v>
       </c>
       <c r="B44" s="132"/>
       <c r="C44" s="149"/>
@@ -7637,9 +7766,9 @@
       <c r="G44" s="130"/>
       <c r="H44" s="148"/>
     </row>
-    <row r="45" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="130" t="s">
-        <v>482</v>
+    <row r="45" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="147" t="s">
+        <v>500</v>
       </c>
       <c r="B45" s="132"/>
       <c r="C45" s="149"/>
@@ -7655,9 +7784,9 @@
       <c r="G45" s="130"/>
       <c r="H45" s="148"/>
     </row>
-    <row r="46" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="130" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B46" s="132"/>
       <c r="C46" s="149"/>
@@ -7673,9 +7802,9 @@
       <c r="G46" s="130"/>
       <c r="H46" s="148"/>
     </row>
-    <row r="47" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="130" t="s">
-        <v>268</v>
+    <row r="47" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="147" t="s">
+        <v>593</v>
       </c>
       <c r="B47" s="132"/>
       <c r="C47" s="149"/>
@@ -7691,9 +7820,9 @@
       <c r="G47" s="130"/>
       <c r="H47" s="148"/>
     </row>
-    <row r="48" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="130" t="s">
-        <v>41</v>
+    <row r="48" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="147" t="s">
+        <v>574</v>
       </c>
       <c r="B48" s="132"/>
       <c r="C48" s="149"/>
@@ -7709,9 +7838,9 @@
       <c r="G48" s="130"/>
       <c r="H48" s="148"/>
     </row>
-    <row r="49" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="130" t="s">
-        <v>273</v>
+    <row r="49" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="147" t="s">
+        <v>178</v>
       </c>
       <c r="B49" s="132"/>
       <c r="C49" s="149"/>
@@ -7727,9 +7856,9 @@
       <c r="G49" s="130"/>
       <c r="H49" s="148"/>
     </row>
-    <row r="50" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="130" t="s">
-        <v>129</v>
+    <row r="50" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="147" t="s">
+        <v>576</v>
       </c>
       <c r="B50" s="132"/>
       <c r="C50" s="149"/>
@@ -7745,9 +7874,9 @@
       <c r="G50" s="130"/>
       <c r="H50" s="148"/>
     </row>
-    <row r="51" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="130" t="s">
-        <v>274</v>
+    <row r="51" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="147" t="s">
+        <v>541</v>
       </c>
       <c r="B51" s="132"/>
       <c r="C51" s="149"/>
@@ -7763,9 +7892,9 @@
       <c r="G51" s="130"/>
       <c r="H51" s="148"/>
     </row>
-    <row r="52" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="130" t="s">
-        <v>21</v>
+    <row r="52" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="147" t="s">
+        <v>239</v>
       </c>
       <c r="B52" s="132"/>
       <c r="C52" s="149"/>
@@ -7781,9 +7910,9 @@
       <c r="G52" s="130"/>
       <c r="H52" s="148"/>
     </row>
-    <row r="53" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="130" t="s">
-        <v>36</v>
+        <v>492</v>
       </c>
       <c r="B53" s="132"/>
       <c r="C53" s="149"/>
@@ -7799,9 +7928,9 @@
       <c r="G53" s="130"/>
       <c r="H53" s="148"/>
     </row>
-    <row r="54" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="130" t="s">
-        <v>256</v>
+        <v>482</v>
       </c>
       <c r="B54" s="132"/>
       <c r="C54" s="149"/>
@@ -7817,9 +7946,9 @@
       <c r="G54" s="130"/>
       <c r="H54" s="148"/>
     </row>
-    <row r="55" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="130" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B55" s="132"/>
       <c r="C55" s="149"/>
@@ -7835,196 +7964,331 @@
       <c r="G55" s="130"/>
       <c r="H55" s="148"/>
     </row>
-    <row r="56" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="150" t="s">
+    <row r="56" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="130" t="s">
+        <v>268</v>
+      </c>
+      <c r="B56" s="132"/>
+      <c r="C56" s="149"/>
+      <c r="D56" s="138"/>
+      <c r="E56" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F56" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G56" s="130"/>
+      <c r="H56" s="148"/>
+    </row>
+    <row r="57" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="130" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="132"/>
+      <c r="C57" s="149"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F57" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G57" s="130"/>
+      <c r="H57" s="148"/>
+    </row>
+    <row r="58" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="130" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58" s="132"/>
+      <c r="C58" s="149"/>
+      <c r="D58" s="138"/>
+      <c r="E58" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F58" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G58" s="130"/>
+      <c r="H58" s="148"/>
+    </row>
+    <row r="59" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="132"/>
+      <c r="C59" s="149"/>
+      <c r="D59" s="138"/>
+      <c r="E59" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F59" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G59" s="130"/>
+      <c r="H59" s="148"/>
+    </row>
+    <row r="60" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="130" t="s">
+        <v>274</v>
+      </c>
+      <c r="B60" s="132"/>
+      <c r="C60" s="149"/>
+      <c r="D60" s="138"/>
+      <c r="E60" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F60" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G60" s="130"/>
+      <c r="H60" s="148"/>
+    </row>
+    <row r="61" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="130" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="132"/>
+      <c r="C61" s="149"/>
+      <c r="D61" s="138"/>
+      <c r="E61" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F61" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G61" s="130"/>
+      <c r="H61" s="148"/>
+    </row>
+    <row r="62" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="130" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" s="132"/>
+      <c r="C62" s="149"/>
+      <c r="D62" s="138"/>
+      <c r="E62" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F62" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G62" s="130"/>
+      <c r="H62" s="148"/>
+    </row>
+    <row r="63" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="130" t="s">
+        <v>256</v>
+      </c>
+      <c r="B63" s="132"/>
+      <c r="C63" s="149"/>
+      <c r="D63" s="138"/>
+      <c r="E63" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F63" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G63" s="130"/>
+      <c r="H63" s="148"/>
+    </row>
+    <row r="64" spans="1:8" ht="16.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="130" t="s">
+        <v>259</v>
+      </c>
+      <c r="B64" s="132"/>
+      <c r="C64" s="149"/>
+      <c r="D64" s="138"/>
+      <c r="E64" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F64" s="133" t="e">
+        <f>INDEX(TAB_Leistungen_30[[Tätigkeit]:[Stk.kosten/Kosten bei Stundensatz]],MATCH(TAB_Doku_201910[[#This Row],[Leistung]],TAB_Leistungen_30[Tätigkeit],0),3)*TAB_Doku_201910[[#This Row],[Stk.]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G64" s="130"/>
+      <c r="H64" s="148"/>
+    </row>
+    <row r="65" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="150" t="s">
         <v>491</v>
       </c>
-      <c r="B56" s="151">
+      <c r="B65" s="151">
         <f>SUBTOTAL(5,TAB_Doku_201910[Datum])</f>
         <v>44201</v>
       </c>
-      <c r="C56" s="152">
+      <c r="C65" s="152">
         <f>SUBTOTAL(4,TAB_Doku_201910[Datum])</f>
-        <v>44203</v>
-      </c>
-      <c r="D56" s="153"/>
-      <c r="E56" s="153"/>
-      <c r="F56" s="154" t="e">
+        <v>44210</v>
+      </c>
+      <c r="D65" s="153"/>
+      <c r="E65" s="153"/>
+      <c r="F65" s="154">
         <f>SUBTOTAL(9,TAB_Doku_201910[[Kosten ]])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G56" s="150"/>
-      <c r="H56" s="155"/>
-    </row>
-    <row r="57" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C57"/>
-    </row>
-    <row r="58" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C60"/>
-    </row>
-    <row r="61" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C63"/>
-    </row>
-    <row r="64" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C64"/>
-    </row>
-    <row r="65" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C65"/>
-    </row>
-    <row r="66" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+      <c r="G65" s="150"/>
+      <c r="H65" s="155"/>
+    </row>
+    <row r="66" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66"/>
     </row>
-    <row r="67" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67"/>
     </row>
-    <row r="68" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68"/>
     </row>
-    <row r="69" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69"/>
     </row>
-    <row r="70" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70"/>
     </row>
-    <row r="71" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71"/>
     </row>
-    <row r="72" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72"/>
     </row>
-    <row r="73" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73"/>
     </row>
-    <row r="74" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74"/>
     </row>
-    <row r="75" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75"/>
     </row>
-    <row r="76" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76"/>
     </row>
-    <row r="77" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77"/>
     </row>
-    <row r="78" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78"/>
     </row>
-    <row r="79" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79"/>
     </row>
-    <row r="80" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C80"/>
     </row>
-    <row r="81" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C81"/>
     </row>
-    <row r="82" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C82"/>
     </row>
-    <row r="83" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C83"/>
     </row>
-    <row r="84" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C84"/>
     </row>
-    <row r="85" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C85"/>
     </row>
-    <row r="86" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C86"/>
     </row>
-    <row r="87" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C87"/>
     </row>
-    <row r="88" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C88"/>
     </row>
-    <row r="89" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C89"/>
     </row>
-    <row r="90" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C90"/>
     </row>
-    <row r="91" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C91"/>
     </row>
-    <row r="92" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C92"/>
-      <c r="I92" t="s">
+    </row>
+    <row r="93" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C93"/>
+    </row>
+    <row r="94" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C94"/>
+    </row>
+    <row r="95" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C95"/>
+    </row>
+    <row r="96" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C96"/>
+    </row>
+    <row r="97" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C97"/>
+    </row>
+    <row r="98" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C101"/>
+      <c r="I101" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="93" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C93"/>
-    </row>
-    <row r="94" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C94"/>
-    </row>
-    <row r="95" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C95"/>
-    </row>
-    <row r="96" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C96"/>
-    </row>
-    <row r="97" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C97"/>
-    </row>
-    <row r="98" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C98"/>
-    </row>
-    <row r="99" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C99"/>
-    </row>
-    <row r="100" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C100"/>
-    </row>
-    <row r="101" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="C101"/>
-    </row>
-    <row r="102" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C102"/>
     </row>
-    <row r="103" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C103"/>
     </row>
-    <row r="104" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C104"/>
     </row>
-    <row r="105" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C105"/>
     </row>
-    <row r="106" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C106"/>
     </row>
-    <row r="107" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C107"/>
     </row>
-    <row r="108" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C108"/>
     </row>
-    <row r="109" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C109"/>
     </row>
-    <row r="110" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C110"/>
     </row>
-    <row r="111" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C111"/>
     </row>
-    <row r="112" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C112"/>
     </row>
     <row r="113" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -8090,15 +8354,8 @@
     <row r="133" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C133"/>
     </row>
-    <row r="134" spans="1:8" s="143" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A134"/>
-      <c r="B134"/>
+    <row r="134" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C134"/>
-      <c r="D134"/>
-      <c r="E134"/>
-      <c r="F134"/>
-      <c r="G134"/>
-      <c r="H134"/>
     </row>
     <row r="135" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C135"/>
@@ -8112,15 +8369,8 @@
     <row r="138" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C138"/>
     </row>
-    <row r="139" spans="1:8" s="143" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A139"/>
-      <c r="B139"/>
+    <row r="139" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C139"/>
-      <c r="D139"/>
-      <c r="E139"/>
-      <c r="F139"/>
-      <c r="G139"/>
-      <c r="H139"/>
     </row>
     <row r="140" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C140"/>
@@ -8131,61 +8381,75 @@
     <row r="142" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C142"/>
     </row>
-    <row r="143" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" s="143" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A143"/>
+      <c r="B143"/>
       <c r="C143"/>
+      <c r="D143"/>
+      <c r="E143"/>
+      <c r="F143"/>
+      <c r="G143"/>
+      <c r="H143"/>
     </row>
     <row r="144" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C144"/>
     </row>
-    <row r="145" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C145"/>
     </row>
-    <row r="146" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C146"/>
     </row>
-    <row r="147" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C147"/>
     </row>
-    <row r="148" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" s="143" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A148"/>
+      <c r="B148"/>
       <c r="C148"/>
-    </row>
-    <row r="149" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D148"/>
+      <c r="E148"/>
+      <c r="F148"/>
+      <c r="G148"/>
+      <c r="H148"/>
+    </row>
+    <row r="149" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C149"/>
     </row>
-    <row r="150" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C150"/>
     </row>
-    <row r="151" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C151"/>
     </row>
-    <row r="152" spans="3:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C152"/>
     </row>
-    <row r="153" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C153"/>
     </row>
-    <row r="154" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C154"/>
     </row>
-    <row r="155" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C155"/>
     </row>
-    <row r="156" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C156"/>
     </row>
-    <row r="157" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C157"/>
     </row>
-    <row r="158" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C158"/>
     </row>
-    <row r="159" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C159"/>
     </row>
-    <row r="160" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C160"/>
     </row>
-    <row r="161" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C161"/>
     </row>
     <row r="162" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -8200,7 +8464,7 @@
     <row r="165" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C165"/>
     </row>
-    <row r="166" spans="3:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C166"/>
     </row>
     <row r="167" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -8227,7 +8491,7 @@
     <row r="174" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C174"/>
     </row>
-    <row r="175" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:3" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C175"/>
     </row>
     <row r="176" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -8638,11 +8902,38 @@
     <row r="311" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C311"/>
     </row>
-    <row r="312" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C312"/>
     </row>
-    <row r="313" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C313"/>
+    </row>
+    <row r="314" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C314"/>
+    </row>
+    <row r="315" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C315"/>
+    </row>
+    <row r="316" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C316"/>
+    </row>
+    <row r="317" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C317"/>
+    </row>
+    <row r="318" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C318"/>
+    </row>
+    <row r="319" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C319"/>
+    </row>
+    <row r="320" spans="3:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C320"/>
+    </row>
+    <row r="321" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C321"/>
+    </row>
+    <row r="322" spans="3:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C322"/>
     </row>
   </sheetData>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.47244094488188981" bottom="0.47244094488188981" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8661,7 +8952,7 @@
           <x14:formula1>
             <xm:f>'Leistungen-Liste'!$F$1:$F$39</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B55</xm:sqref>
+          <xm:sqref>B2:B64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8677,10 +8968,10 @@
   <dimension ref="A1:I314"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F318" sqref="F318"/>
+      <selection pane="bottomRight" activeCell="A314" sqref="A314:XFD314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8690,7 +8981,8 @@
     <col min="3" max="3" width="13.77734375" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.21875" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="7" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" customWidth="1"/>
     <col min="8" max="8" width="80.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8742,7 +9034,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H2" s="134" t="s">
         <v>838</v>
@@ -8770,7 +9062,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H3" s="134" t="s">
         <v>838</v>
@@ -8798,7 +9090,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H4" s="134" t="s">
         <v>838</v>
@@ -8826,7 +9118,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H5" s="134" t="s">
         <v>837</v>
@@ -8854,7 +9146,7 @@
         <v>120</v>
       </c>
       <c r="G6" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H6" s="134" t="s">
         <v>834</v>
@@ -8882,7 +9174,7 @@
         <v>7.5</v>
       </c>
       <c r="G7" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H7" s="134" t="s">
         <v>833</v>
@@ -8910,7 +9202,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H8" s="134" t="s">
         <v>836</v>
@@ -8938,7 +9230,7 @@
         <v>60</v>
       </c>
       <c r="G9" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H9" s="134" t="s">
         <v>835</v>
@@ -8966,7 +9258,7 @@
         <v>7.5</v>
       </c>
       <c r="G10" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H10" s="134" t="s">
         <v>832</v>
@@ -8994,7 +9286,7 @@
         <v>7.5</v>
       </c>
       <c r="G11" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H11" s="134" t="s">
         <v>831</v>
@@ -9022,7 +9314,7 @@
         <v>7.5</v>
       </c>
       <c r="G12" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H12" s="134" t="s">
         <v>829</v>
@@ -9050,7 +9342,7 @@
         <v>30</v>
       </c>
       <c r="G13" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H13" s="134" t="s">
         <v>825</v>
@@ -9078,7 +9370,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H14" s="134" t="s">
         <v>824</v>
@@ -9106,7 +9398,7 @@
         <v>7.5</v>
       </c>
       <c r="G15" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H15" s="134" t="s">
         <v>823</v>
@@ -9134,7 +9426,7 @@
         <v>7.5</v>
       </c>
       <c r="G16" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H16" s="134" t="s">
         <v>821</v>
@@ -9162,7 +9454,7 @@
         <v>7.5</v>
       </c>
       <c r="G17" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H17" s="134" t="s">
         <v>820</v>
@@ -9190,7 +9482,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H18" s="134" t="s">
         <v>827</v>
@@ -9218,7 +9510,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H19" s="134" t="s">
         <v>817</v>
@@ -9246,7 +9538,7 @@
         <v>7.5</v>
       </c>
       <c r="G20" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H20" s="134" t="s">
         <v>815</v>
@@ -9274,7 +9566,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H21" s="134" t="s">
         <v>826</v>
@@ -9302,7 +9594,7 @@
         <v>7.5</v>
       </c>
       <c r="G22" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H22" s="134" t="s">
         <v>818</v>
@@ -9330,7 +9622,7 @@
         <v>7.5</v>
       </c>
       <c r="G23" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H23" s="134" t="s">
         <v>814</v>
@@ -9358,7 +9650,7 @@
         <v>7.5</v>
       </c>
       <c r="G24" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H24" s="134" t="s">
         <v>822</v>
@@ -9386,7 +9678,7 @@
         <v>7.5</v>
       </c>
       <c r="G25" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H25" s="134" t="s">
         <v>812</v>
@@ -9414,7 +9706,7 @@
         <v>7.5</v>
       </c>
       <c r="G26" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H26" s="134" t="s">
         <v>828</v>
@@ -9442,7 +9734,7 @@
         <v>15</v>
       </c>
       <c r="G27" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H27" s="134" t="s">
         <v>809</v>
@@ -9470,7 +9762,7 @@
         <v>7.5</v>
       </c>
       <c r="G28" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H28" s="134" t="s">
         <v>806</v>
@@ -9498,7 +9790,7 @@
         <v>7.5</v>
       </c>
       <c r="G29" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H29" s="134" t="s">
         <v>803</v>
@@ -9526,7 +9818,7 @@
         <v>15</v>
       </c>
       <c r="G30" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H30" s="134" t="s">
         <v>811</v>
@@ -9554,7 +9846,7 @@
         <v>5</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H31" s="134" t="s">
         <v>808</v>
@@ -9582,7 +9874,7 @@
         <v>7.5</v>
       </c>
       <c r="G32" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H32" s="134" t="s">
         <v>804</v>
@@ -9610,7 +9902,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H33" s="134" t="s">
         <v>807</v>
@@ -9638,7 +9930,7 @@
         <v>90</v>
       </c>
       <c r="G34" s="78" t="s">
-        <v>498</v>
+        <v>846</v>
       </c>
       <c r="H34" s="133" t="s">
         <v>805</v>
@@ -17513,7 +17805,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.47244094488188981" bottom="0.47244094488188981" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L &amp;F&amp;C&amp;A&amp;R&amp;D</oddHeader>
     <oddFooter>&amp;C&amp;P von &amp;N</oddFooter>
@@ -23257,122 +23549,122 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="C2:C90 C94:C123">
-    <cfRule type="containsText" dxfId="23" priority="33" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C15">
-    <cfRule type="containsText" dxfId="22" priority="32" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="21" priority="31" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:C43 C45:C46">
-    <cfRule type="containsText" dxfId="20" priority="30" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C34">
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73:D76 D2:D71">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77:D78">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D81">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="20" priority="14" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89:C90">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C125:C126">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C124">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C128">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C128)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C129">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",C129)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>